<commit_message>
feat: ChangeLog in Title
</commit_message>
<xml_diff>
--- a/ChemicalSummon/Assets/StreamingAssets/TranslatableSentence.xlsx
+++ b/ChemicalSummon/Assets/StreamingAssets/TranslatableSentence.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="3"/>
+    <workbookView windowWidth="22368" windowHeight="9420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="4" r:id="rId1"/>
     <sheet name="Match" sheetId="1" r:id="rId2"/>
     <sheet name="MatchGuide" sheetId="5" r:id="rId3"/>
     <sheet name="Map" sheetId="7" r:id="rId4"/>
-    <sheet name="Other" sheetId="6" r:id="rId5"/>
+    <sheet name="ChangeLog" sheetId="8" r:id="rId5"/>
+    <sheet name="Other" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="189">
   <si>
     <t>ScriptableObjectName</t>
   </si>
@@ -203,9 +204,21 @@
     <t>TurnEnd</t>
   </si>
   <si>
+    <t>回合结束</t>
+  </si>
+  <si>
+    <t>ターンエンド</t>
+  </si>
+  <si>
     <t>StartAttack</t>
   </si>
   <si>
+    <t>开始攻击</t>
+  </si>
+  <si>
+    <t>攻撃開始</t>
+  </si>
+  <si>
     <t>PlayerBlock</t>
   </si>
   <si>
@@ -564,6 +577,22 @@
   </si>
   <si>
     <t>反応式をクリック</t>
+  </si>
+  <si>
+    <t>ChangeLog</t>
+  </si>
+  <si>
+    <t>当前游戏为内测版!
+- 敌人未习得反击融合
+- 燃烧/电击伤害未实装
+* 作品中图片均未授权使用
+请不要二次转载!</t>
+  </si>
+  <si>
+    <t>この作品はアルファテスト中です！
+・敵はカウンターしてきません
+・燃焼/電撃が未実装です
+* 作品中のグラフィックは全て無断で使用しています。2次配布はご遠慮ください！</t>
   </si>
 </sst>
 </file>
@@ -571,10 +600,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -585,16 +614,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,13 +629,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -622,15 +636,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -699,6 +705,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -708,7 +723,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -723,6 +745,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -738,19 +767,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,163 +899,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,21 +972,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -989,15 +1003,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -1019,6 +1024,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1037,10 +1066,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1049,139 +1078,142 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1534,7 +1566,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -1655,8 +1687,8 @@
   <sheetPr/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1808,94 +1840,106 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1938,211 +1982,211 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2157,8 +2201,8 @@
   <sheetPr/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -2185,167 +2229,167 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2356,6 +2400,55 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="40.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="32.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="34.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="109" customHeight="1" spans="1:4">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D1"/>

</xml_diff>